<commit_message>
More complete version of frame, with volcanos changed to 7 degrees.
</commit_message>
<xml_diff>
--- a/layla/parts/Layla_parts_list.xlsx
+++ b/layla/parts/Layla_parts_list.xlsx
@@ -593,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,7 +758,10 @@
       <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <f>SUM(F2:F7)</f>
+        <v>91.16</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -859,7 +862,10 @@
       <c r="E14" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <f>SUM(F9:F13)</f>
+        <v>74.25</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -872,7 +878,10 @@
       <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <f>SUM(F14,F8)</f>
+        <v>165.41</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
@@ -986,7 +995,10 @@
       <c r="E22" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3">
+        <f>SUM(F17:F21)</f>
+        <v>22.700000000000003</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1110,13 +1122,15 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F31" s="3"/>
+      <c r="F31" s="3">
+        <f>SUM(F2:F15)+SUM(F17:F22)+SUM(F26:F30)+F2</f>
+        <v>751.01</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">

</xml_diff>